<commit_message>
Updating and adding initialization rules and functions (see policy group Testbed...).
Edited excel file to include correct naming.
Edited Testbed_Input_IC DMI to include correct naming convention.
</commit_message>
<xml_diff>
--- a/Input Data/Historical_Diversions.xlsx
+++ b/Input Data/Historical_Diversions.xlsx
@@ -39,229 +39,229 @@
     <t>TunnelDiversionBelowCrystalForAg.Diversion Requested</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.AzPumpersAbvImp</t>
+    <t>acre-feet</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.AzPumpersBlwImp</t>
+    <t>Arizona_CU_Schedule.AzPumpersAbvImp</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.AzPumpersDvsToPkr</t>
+    <t>Arizona_CU_Schedule.AzPumpersBlwImp</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.BlmPumpersAbvImp</t>
+    <t>Arizona_CU_Schedule.AzPumpersDvsToPkr</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.BlmPumpersBlwImp</t>
+    <t>Arizona_CU_Schedule.BlmPumpersAbvImp</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.BrookeWater</t>
+    <t>Arizona_CU_Schedule.BlmPumpersBlwImp</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.BullheadCity</t>
+    <t>Arizona_CU_Schedule.BrookeWater</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.CAP</t>
+    <t>Arizona_CU_Schedule.BullheadCity</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.CibolaNWR</t>
+    <t>Arizona_CU_Schedule.CAP</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.CibolaValleyIID</t>
+    <t>Arizona_CU_Schedule.CibolaNWR</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.City of Parker</t>
+    <t>Arizona_CU_Schedule.CibolaValleyIID</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.City of Yuma</t>
+    <t>Arizona_CU_Schedule.City of Parker</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.Cocopah Indian Res</t>
+    <t>Arizona_CU_Schedule.City of Yuma</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.CRIRAz</t>
+    <t>Arizona_CU_Schedule.Cocopah Indian Res</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.DavisDamProject</t>
+    <t>Arizona_CU_Schedule.CRIRAz</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.DesertLawnMemorial</t>
+    <t>Arizona_CU_Schedule.DavisDamProject</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.Ehrenberg</t>
+    <t>Arizona_CU_Schedule.DesertLawnMemorial</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.Ft Yuma</t>
+    <t>Arizona_CU_Schedule.Ehrenberg</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.FtMohaveAz</t>
+    <t>Arizona_CU_Schedule.Ft Yuma</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.Gila Monster Farms</t>
+    <t>Arizona_CU_Schedule.FtMohaveAz</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.GoldenShores</t>
+    <t>Arizona_CU_Schedule.Gila Monster Farms</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.HavasuNWR</t>
+    <t>Arizona_CU_Schedule.GoldenShores</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.ImperialNWR</t>
+    <t>Arizona_CU_Schedule.HavasuNWR</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.LakeHavasuCity</t>
+    <t>Arizona_CU_Schedule.ImperialNWR</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.LMNRA Az Mead</t>
+    <t>Arizona_CU_Schedule.LakeHavasuCity</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.LMNRA Az Mohave</t>
+    <t>Arizona_CU_Schedule.LMNRA Az Mead</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.MCAirStation</t>
+    <t>Arizona_CU_Schedule.LMNRA Az Mohave</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.MohaveValleyIID</t>
+    <t>Arizona_CU_Schedule.MCAirStation</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.MohaveWaterConsDist</t>
+    <t>Arizona_CU_Schedule.MohaveValleyIID</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.NGVIDD</t>
+    <t>Arizona_CU_Schedule.MohaveWaterConsDist</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.SouthernPacific</t>
+    <t>Arizona_CU_Schedule.NGVIDD</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.UnitB</t>
+    <t>Arizona_CU_Schedule.SouthernPacific</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.UofA</t>
+    <t>Arizona_CU_Schedule.UnitB</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.WMIDD</t>
+    <t>Arizona_CU_Schedule.UofA</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.YAO</t>
+    <t>Arizona_CU_Schedule.WMIDD</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.YCWUA</t>
+    <t>Arizona_CU_Schedule.YAO</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.YID</t>
+    <t>Arizona_CU_Schedule.YCWUA</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.YMIDD</t>
+    <t>Arizona_CU_Schedule.YID</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.YumaProvingGround</t>
+    <t>Arizona_CU_Schedule.YMIDD</t>
   </si>
   <si>
-    <t>Arizona_CU_Actual.YumaUnionHighScl</t>
+    <t>Arizona_CU_Schedule.YumaProvingGround</t>
   </si>
   <si>
-    <t>California_CU_Actual.CaPumpersAbvImp</t>
+    <t>Arizona_CU_Schedule.YumaUnionHighScl</t>
   </si>
   <si>
-    <t>California_CU_Actual.Chemehuevi</t>
+    <t>California_CU_Schedule.CaPumpersAbvImp</t>
   </si>
   <si>
-    <t>California_CU_Actual.Coachella</t>
+    <t>California_CU_Schedule.Chemehuevi</t>
   </si>
   <si>
-    <t>California_CU_Actual.CRIRCa</t>
+    <t>California_CU_Schedule.Coachella</t>
   </si>
   <si>
-    <t>California_CU_Actual.FtMohaveCa</t>
+    <t>California_CU_Schedule.CRIRCa</t>
   </si>
   <si>
-    <t>California_CU_Actual.IID</t>
+    <t>California_CU_Schedule.FtMohaveCa</t>
   </si>
   <si>
-    <t>California_CU_Actual.MWD</t>
+    <t>California_CU_Schedule.IID</t>
   </si>
   <si>
-    <t>California_CU_Actual.MWDDiversion</t>
+    <t>California_CU_Schedule.MWD</t>
   </si>
   <si>
-    <t>California_CU_Actual.MWDReturns</t>
+    <t>California_CU_Schedule.MWDDiversion</t>
   </si>
   <si>
-    <t>California_CU_Actual.Needles</t>
+    <t>California_CU_Schedule.MWDReturns</t>
   </si>
   <si>
-    <t>California_CU_Actual.OtherLCWSP</t>
+    <t>California_CU_Schedule.Needles</t>
   </si>
   <si>
-    <t>California_CU_Actual.PaloVerde</t>
+    <t>California_CU_Schedule.OtherLCWSP</t>
   </si>
   <si>
-    <t>California_CU_Actual.Ranch5</t>
+    <t>California_CU_Schedule.PaloVerde</t>
   </si>
   <si>
-    <t>California_CU_Actual.SaltonSea</t>
+    <t>California_CU_Schedule.Ranch5</t>
   </si>
   <si>
-    <t>California_CU_Actual.Winterhaven</t>
+    <t>California_CU_Schedule.SaltonSea</t>
   </si>
   <si>
-    <t>California_CU_Actual.YumaIsland</t>
+    <t>California_CU_Schedule.Winterhaven</t>
   </si>
   <si>
-    <t>California_CU_Actual.YumaProject</t>
+    <t>California_CU_Schedule.YumaIsland</t>
   </si>
   <si>
-    <t>Nevada_CU_Actual.BasicManagement</t>
+    <t>California_CU_Schedule.YumaProject</t>
   </si>
   <si>
-    <t>Nevada_CU_Actual.BigBend</t>
+    <t>Nevada_CU_Schedule.BasicManagement</t>
   </si>
   <si>
-    <t>Nevada_CU_Actual.BoulderCanyonProject</t>
+    <t>Nevada_CU_Schedule.BigBend</t>
   </si>
   <si>
-    <t>Nevada_CU_Actual.City of Henderson</t>
+    <t>Nevada_CU_Schedule.BoulderCanyonProject</t>
   </si>
   <si>
-    <t>Nevada_CU_Actual.FtMohaveNv</t>
+    <t>Nevada_CU_Schedule.City of Henderson</t>
   </si>
   <si>
-    <t>Nevada_CU_Actual.LMNRA Mead</t>
+    <t>Nevada_CU_Schedule.FtMohaveNv</t>
   </si>
   <si>
-    <t>Nevada_CU_Actual.LMNRA Mohave</t>
+    <t>Nevada_CU_Schedule.LMNRA Mead</t>
   </si>
   <si>
-    <t>Nevada_CU_Actual.LVWashReturns</t>
+    <t>Nevada_CU_Schedule.LMNRA Mohave</t>
   </si>
   <si>
-    <t>Nevada_CU_Actual.NvDeptFishGame</t>
+    <t>Nevada_CU_Schedule.LVWashReturns</t>
   </si>
   <si>
-    <t>Nevada_CU_Actual.PacificCoastBuilding</t>
+    <t>Nevada_CU_Schedule.NvDeptFishGame</t>
   </si>
   <si>
-    <t>Nevada_CU_Actual.SCE</t>
+    <t>Nevada_CU_Schedule.PacificCoastBuilding</t>
   </si>
   <si>
-    <t>Nevada_CU_Actual.SNWADiversion</t>
+    <t>Nevada_CU_Schedule.SCE</t>
   </si>
   <si>
-    <t>Nevada_CU_Actual.SNWP</t>
+    <t>Nevada_CU_Schedule.SNWADiversion</t>
   </si>
   <si>
-    <t>Mexico_CU_Actual.MexicoBypass</t>
+    <t>Nevada_CU_Schedule.SNWP</t>
   </si>
   <si>
-    <t>Mexico_CU_Actual.MexicoExcess</t>
+    <t>Mexico_CU_Schedule.MexicoBypass</t>
   </si>
   <si>
-    <t>Mexico_CU_Actual.MexicoSched</t>
+    <t>Mexico_CU_Schedule.MexicoExcess</t>
   </si>
   <si>
-    <t>Mexico_CU_Actual.MexicoTJ</t>
+    <t>Mexico_CU_Schedule.MexicoSched</t>
   </si>
   <si>
-    <t>acre-feet</t>
+    <t>Mexico_CU_Schedule.MexicoTJ</t>
   </si>
 </sst>
 </file>
@@ -587,7 +587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E482"/>
   <sheetViews>
-    <sheetView topLeftCell="A442" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -7394,450 +7394,450 @@
   <sheetData>
     <row r="1" spans="1:75" s="2" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AD1" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AE1" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AF1" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AG1" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AH1" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AI1" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AJ1" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AK1" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AL1" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AM1" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AN1" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AO1" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AP1" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AQ1" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AR1" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AS1" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AT1" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AU1" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AV1" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AW1" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AX1" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AY1" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AZ1" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="BA1" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="BB1" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="BC1" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="BD1" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="BE1" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BF1" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="BG1" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="BH1" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="BI1" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="BJ1" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="BK1" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="BL1" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="BM1" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="BN1" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="BO1" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="BP1" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="BQ1" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="BR1" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="BS1" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="BT1" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="BU1" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="BV1" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="BW1" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:75" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="I2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="J2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="K2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="L2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="M2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="N2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="O2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="P2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="Q2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="R2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="S2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="T2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="U2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="V2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="W2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="X2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="Y2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="Z2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AA2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AB2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AC2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AD2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AE2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AF2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AG2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AH2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AI2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AJ2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AK2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AL2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AM2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AN2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AO2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AP2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AQ2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AR2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AS2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AT2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AU2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AV2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AW2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AX2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AY2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AZ2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="BA2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="BB2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="BC2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="BD2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="BE2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="BF2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="BG2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="BH2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="BI2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="BJ2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="BK2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="BL2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="BM2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="BN2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="BO2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="BP2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="BQ2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="BR2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="BS2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="BT2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="BU2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="BV2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="BW2" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:75" x14ac:dyDescent="0.35">

</xml_diff>